<commit_message>
Created version 3 of direct GF calculation; switched script-like organization to functional.
</commit_message>
<xml_diff>
--- a/python/TimingData.xlsx
+++ b/python/TimingData.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14000" yWindow="4640" windowWidth="34400" windowHeight="24500" tabRatio="500"/>
+    <workbookView xWindow="11320" yWindow="160" windowWidth="34400" windowHeight="24500" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="AllGFs" sheetId="1" r:id="rId1"/>
+    <sheet name="RelevantOnlyGFs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
   <si>
     <t>N (sites)</t>
   </si>
@@ -109,8 +110,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -169,7 +182,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="55">
+  <cellStyles count="67">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -197,6 +210,12 @@
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -224,6 +243,12 @@
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -282,7 +307,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$5</c:f>
+              <c:f>AllGFs!$D$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -313,7 +338,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$5:$A$15</c:f>
+              <c:f>AllGFs!$A$5:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -355,7 +380,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$5:$E$15</c:f>
+              <c:f>AllGFs!$E$5:$E$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -402,7 +427,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$17</c:f>
+              <c:f>AllGFs!$D$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -432,7 +457,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$17:$A$21</c:f>
+              <c:f>AllGFs!$A$17:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -456,7 +481,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$17:$E$21</c:f>
+              <c:f>AllGFs!$E$17:$E$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -592,7 +617,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$5</c:f>
+              <c:f>AllGFs!$D$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -623,7 +648,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$5:$A$15</c:f>
+              <c:f>AllGFs!$A$5:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -665,7 +690,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$5:$G$15</c:f>
+              <c:f>AllGFs!$G$5:$G$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -712,7 +737,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$17</c:f>
+              <c:f>AllGFs!$D$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -737,7 +762,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$17:$A$21</c:f>
+              <c:f>AllGFs!$A$17:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -761,7 +786,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$17:$G$21</c:f>
+              <c:f>AllGFs!$G$17:$G$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -897,7 +922,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$5</c:f>
+              <c:f>AllGFs!$D$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -928,7 +953,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$5:$A$15</c:f>
+              <c:f>AllGFs!$A$5:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -970,7 +995,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$J$5:$J$15</c:f>
+              <c:f>AllGFs!$J$5:$J$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1124,7 +1149,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$5</c:f>
+              <c:f>AllGFs!$D$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1155,7 +1180,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$5:$A$15</c:f>
+              <c:f>AllGFs!$A$5:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1197,7 +1222,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$K$5:$K$15</c:f>
+              <c:f>AllGFs!$K$5:$K$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1286,6 +1311,1119 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="2116924136"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>GF Calculation Wall Time</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>RelevantOnlyGFs!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>216</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="4"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.26676006122784"/>
+                  <c:y val="0.120863953781215"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>RelevantOnlyGFs!$A$4:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>120.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>130.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>RelevantOnlyGFs!$G$4:$G$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.0576801</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0649681</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0846879</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.114576</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.264376</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.487881</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.881097</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.49757</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.80097</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12.4413</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>18.9238</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2116285512"/>
+        <c:axId val="2118091400"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2116285512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Lattice Size, N</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2118091400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2118091400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2116285512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Diagonalization Wall Time</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>RelevantOnlyGFs!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>216</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="4"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.15228943961089"/>
+                  <c:y val="-0.0417490116007994"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>RelevantOnlyGFs!$A$4:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>120.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>130.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>RelevantOnlyGFs!$H$4:$H$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.000128031</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.000946045</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.026684</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.163176</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.636186</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.07382</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.46896</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.7608</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>91.68940000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>280.094</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>453.037</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2120773768"/>
+        <c:axId val="2118243800"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2120773768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Lattice Size, N</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.420844429544557"/>
+              <c:y val="0.937974717546003"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2118243800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2118243800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2120773768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Program Wall Time</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>RelevantOnlyGFs!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>216</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="4"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.15228943961089"/>
+                  <c:y val="-0.0417490116007994"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>RelevantOnlyGFs!$A$4:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>120.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>130.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>RelevantOnlyGFs!$F$4:$F$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.116971</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.13506</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.249129</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.602958</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.69721</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.34716</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.92269</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20.7832</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>124.155</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>347.923</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>548.279</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2121216360"/>
+        <c:axId val="2121221496"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2121216360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Lattice Size, N</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2121221496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2121221496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2121216360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Memory Requirements</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>RelevantOnlyGFs!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>216</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.15228943961089"/>
+                  <c:y val="-0.0417490116007994"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>RelevantOnlyGFs!$A$4:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>120.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>130.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>RelevantOnlyGFs!$E$4:$E$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.042</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.044</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.047</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.07</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.082</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.133</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.322</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.16</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2120055688"/>
+        <c:axId val="2120060520"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2120055688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Lattice Size, N</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2120060520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2120060520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>GB</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2120055688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1419,6 +2557,139 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>58058</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>370115</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>166916</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>137886</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>762001</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>72575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>29029</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1117600</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>101604</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1001485</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>159656</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>420914</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>43545</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -1762,8 +3033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2446,4 +3717,582 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="5" max="5" width="12.1640625" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <f>A4</f>
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <f>A4</f>
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <f>(5.5-0.1)/0.025</f>
+        <v>216</v>
+      </c>
+      <c r="E4">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="F4">
+        <v>0.11697100000000001</v>
+      </c>
+      <c r="G4">
+        <v>5.7680099999999998E-2</v>
+      </c>
+      <c r="H4">
+        <v>1.2803099999999999E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <f>A5</f>
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <f>A5</f>
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <f>(5.5-0.1)/0.025</f>
+        <v>216</v>
+      </c>
+      <c r="E5">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="F5">
+        <v>0.13506000000000001</v>
+      </c>
+      <c r="G5">
+        <v>6.4968100000000001E-2</v>
+      </c>
+      <c r="H5">
+        <v>9.4604499999999996E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <f>A6</f>
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <f>A6</f>
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <f>(5.5-0.1)/0.025</f>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <f>A7</f>
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <f>A7</f>
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <f>(5.5-0.1)/0.025</f>
+        <v>216</v>
+      </c>
+      <c r="E7">
+        <v>4.7E-2</v>
+      </c>
+      <c r="F7">
+        <v>0.24912899999999999</v>
+      </c>
+      <c r="G7">
+        <v>8.4687899999999997E-2</v>
+      </c>
+      <c r="H7">
+        <v>2.6683999999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8">
+        <v>25</v>
+      </c>
+      <c r="B8">
+        <f>A8</f>
+        <v>25</v>
+      </c>
+      <c r="C8">
+        <f>A8</f>
+        <v>25</v>
+      </c>
+      <c r="D8">
+        <f>(5.5-0.1)/0.025</f>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9">
+        <v>30</v>
+      </c>
+      <c r="B9">
+        <f>A9</f>
+        <v>30</v>
+      </c>
+      <c r="C9">
+        <f>A9</f>
+        <v>30</v>
+      </c>
+      <c r="D9">
+        <f>(5.5-0.1)/0.025</f>
+        <v>216</v>
+      </c>
+      <c r="E9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F9">
+        <v>0.60295799999999999</v>
+      </c>
+      <c r="G9">
+        <v>0.114576</v>
+      </c>
+      <c r="H9">
+        <v>0.16317599999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10">
+        <v>35</v>
+      </c>
+      <c r="B10">
+        <f>A10</f>
+        <v>35</v>
+      </c>
+      <c r="C10">
+        <f>A10</f>
+        <v>35</v>
+      </c>
+      <c r="D10">
+        <f>(5.5-0.1)/0.025</f>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11">
+        <v>40</v>
+      </c>
+      <c r="B11">
+        <f>A11</f>
+        <v>40</v>
+      </c>
+      <c r="C11">
+        <f>A11</f>
+        <v>40</v>
+      </c>
+      <c r="D11">
+        <f>(5.5-0.1)/0.025</f>
+        <v>216</v>
+      </c>
+      <c r="E11">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="F11">
+        <v>1.6972100000000001</v>
+      </c>
+      <c r="G11">
+        <v>0.264376</v>
+      </c>
+      <c r="H11">
+        <v>0.63618600000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12">
+        <v>45</v>
+      </c>
+      <c r="B12">
+        <f>A12</f>
+        <v>45</v>
+      </c>
+      <c r="C12">
+        <f>A12</f>
+        <v>45</v>
+      </c>
+      <c r="D12">
+        <f>(5.5-0.1)/0.025</f>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13">
+        <v>50</v>
+      </c>
+      <c r="B13">
+        <f>A13</f>
+        <v>50</v>
+      </c>
+      <c r="C13">
+        <f>A13</f>
+        <v>50</v>
+      </c>
+      <c r="D13">
+        <f>(5.5-0.1)/0.025</f>
+        <v>216</v>
+      </c>
+      <c r="E13">
+        <v>0.12</v>
+      </c>
+      <c r="F13">
+        <v>4.3471599999999997</v>
+      </c>
+      <c r="G13">
+        <v>0.48788100000000001</v>
+      </c>
+      <c r="H13">
+        <v>2.07382</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14">
+        <v>60</v>
+      </c>
+      <c r="B14">
+        <f>A14</f>
+        <v>60</v>
+      </c>
+      <c r="C14">
+        <f>A14</f>
+        <v>60</v>
+      </c>
+      <c r="D14">
+        <f>(5.5-0.1)/0.025</f>
+        <v>216</v>
+      </c>
+      <c r="E14">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="F14">
+        <v>9.9226899999999993</v>
+      </c>
+      <c r="G14">
+        <v>0.88109700000000002</v>
+      </c>
+      <c r="H14">
+        <v>5.46896</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15">
+        <v>70</v>
+      </c>
+      <c r="B15">
+        <f>A15</f>
+        <v>70</v>
+      </c>
+      <c r="C15">
+        <f>A15</f>
+        <v>70</v>
+      </c>
+      <c r="D15">
+        <f>(5.5-0.1)/0.025</f>
+        <v>216</v>
+      </c>
+      <c r="E15">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="F15">
+        <v>20.783200000000001</v>
+      </c>
+      <c r="G15">
+        <v>1.4975700000000001</v>
+      </c>
+      <c r="H15">
+        <v>12.7608</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16">
+        <v>100</v>
+      </c>
+      <c r="B16">
+        <f>A16</f>
+        <v>100</v>
+      </c>
+      <c r="C16">
+        <f>A16</f>
+        <v>100</v>
+      </c>
+      <c r="D16">
+        <f>(5.5-0.1)/0.025</f>
+        <v>216</v>
+      </c>
+      <c r="E16">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="F16">
+        <v>124.155</v>
+      </c>
+      <c r="G16">
+        <v>5.8009700000000004</v>
+      </c>
+      <c r="H16">
+        <v>91.689400000000006</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17">
+        <v>120</v>
+      </c>
+      <c r="B17">
+        <f>A17</f>
+        <v>120</v>
+      </c>
+      <c r="C17">
+        <f>A17</f>
+        <v>120</v>
+      </c>
+      <c r="D17">
+        <f>(5.5-0.1)/0.025</f>
+        <v>216</v>
+      </c>
+      <c r="E17">
+        <v>2.35</v>
+      </c>
+      <c r="F17">
+        <v>347.923</v>
+      </c>
+      <c r="G17">
+        <v>12.4413</v>
+      </c>
+      <c r="H17">
+        <v>280.09399999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18">
+        <v>130</v>
+      </c>
+      <c r="B18">
+        <f>A18</f>
+        <v>130</v>
+      </c>
+      <c r="C18">
+        <f>A18</f>
+        <v>130</v>
+      </c>
+      <c r="D18">
+        <f>(5.5-0.1)/0.025</f>
+        <v>216</v>
+      </c>
+      <c r="F18">
+        <v>548.279</v>
+      </c>
+      <c r="G18">
+        <v>18.9238</v>
+      </c>
+      <c r="H18">
+        <v>453.03699999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19">
+        <v>150</v>
+      </c>
+      <c r="B19">
+        <f>A19</f>
+        <v>150</v>
+      </c>
+      <c r="C19">
+        <f>A19</f>
+        <v>150</v>
+      </c>
+      <c r="D19">
+        <f>(5.5-0.1)/0.025</f>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21">
+        <f>A21</f>
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <f>A21</f>
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <f>(5.5-0.1)/0.001</f>
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22">
+        <v>10</v>
+      </c>
+      <c r="B22">
+        <f>A22</f>
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <f>A22</f>
+        <v>10</v>
+      </c>
+      <c r="D22">
+        <f>(5.5-0.1)/0.001</f>
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23">
+        <v>15</v>
+      </c>
+      <c r="B23">
+        <f>A23</f>
+        <v>15</v>
+      </c>
+      <c r="C23">
+        <f>A23</f>
+        <v>15</v>
+      </c>
+      <c r="D23">
+        <f>(5.5-0.1)/0.001</f>
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24">
+        <v>20</v>
+      </c>
+      <c r="B24">
+        <f>A24</f>
+        <v>20</v>
+      </c>
+      <c r="C24">
+        <f>A24</f>
+        <v>20</v>
+      </c>
+      <c r="D24">
+        <f>(5.5-0.1)/0.001</f>
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <f>A25</f>
+        <v>25</v>
+      </c>
+      <c r="C25">
+        <f>A25</f>
+        <v>25</v>
+      </c>
+      <c r="D25">
+        <f>(5.5-0.1)/0.001</f>
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26">
+        <v>30</v>
+      </c>
+      <c r="B26">
+        <f>A26</f>
+        <v>30</v>
+      </c>
+      <c r="C26">
+        <f>A26</f>
+        <v>30</v>
+      </c>
+      <c r="D26">
+        <f>(5.5-0.1)/0.001</f>
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="B27">
+        <f>A27</f>
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <f>A27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Wrote initial code to output relevant arrays for later comparison with Ping's code. - JTC
</commit_message>
<xml_diff>
--- a/python/TimingData.xlsx
+++ b/python/TimingData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11320" yWindow="160" windowWidth="34400" windowHeight="24500" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="27720" yWindow="1640" windowWidth="34400" windowHeight="24500" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AllGFs" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>N (sites)</t>
   </si>
@@ -62,6 +62,18 @@
   </si>
   <si>
     <t>NOTE: as the crystal size gets larger, the eigenfunction orthonormality drops. I don't know why.</t>
+  </si>
+  <si>
+    <t>NumDisorders:</t>
+  </si>
+  <si>
+    <t>Estimated Time (s)</t>
+  </si>
+  <si>
+    <t>Estimated Time (min)</t>
+  </si>
+  <si>
+    <t>Estimated Time (hr)</t>
   </si>
 </sst>
 </file>
@@ -513,30 +525,29 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2101452408"/>
-        <c:axId val="2116566024"/>
+        <c:axId val="2063442968"/>
+        <c:axId val="2063448056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2101452408"/>
+        <c:axId val="2063442968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116566024"/>
+        <c:crossAx val="2063448056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2116566024"/>
+        <c:axId val="2063448056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -544,21 +555,19 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2101452408"/>
+        <c:crossAx val="2063442968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -603,7 +612,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -756,7 +764,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -818,30 +825,29 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2115215992"/>
-        <c:axId val="2118182152"/>
+        <c:axId val="2063488744"/>
+        <c:axId val="2063493832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2115215992"/>
+        <c:axId val="2063488744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2118182152"/>
+        <c:crossAx val="2063493832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2118182152"/>
+        <c:axId val="2063493832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -849,21 +855,19 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115215992"/>
+        <c:crossAx val="2063488744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -908,7 +912,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1045,30 +1048,29 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2119066856"/>
-        <c:axId val="2115245080"/>
+        <c:axId val="2063524872"/>
+        <c:axId val="2063529864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2119066856"/>
+        <c:axId val="2063524872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115245080"/>
+        <c:crossAx val="2063529864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2115245080"/>
+        <c:axId val="2063529864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1076,21 +1078,19 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2119066856"/>
+        <c:crossAx val="2063524872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1135,7 +1135,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1272,30 +1271,29 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2116924136"/>
-        <c:axId val="2116865624"/>
+        <c:axId val="2063562280"/>
+        <c:axId val="2063567272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2116924136"/>
+        <c:axId val="2063562280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116865624"/>
+        <c:crossAx val="2063567272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2116865624"/>
+        <c:axId val="2063567272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1303,21 +1301,19 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116924136"/>
+        <c:crossAx val="2063562280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1514,11 +1510,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2116285512"/>
-        <c:axId val="2118091400"/>
+        <c:axId val="2062813512"/>
+        <c:axId val="2062808280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2116285512"/>
+        <c:axId val="2062813512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1547,12 +1543,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2118091400"/>
+        <c:crossAx val="2062808280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2118091400"/>
+        <c:axId val="2062808280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1582,7 +1578,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116285512"/>
+        <c:crossAx val="2062813512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1786,11 +1782,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2120773768"/>
-        <c:axId val="2118243800"/>
+        <c:axId val="2062773320"/>
+        <c:axId val="2062767720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2120773768"/>
+        <c:axId val="2062773320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1833,12 +1829,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2118243800"/>
+        <c:crossAx val="2062767720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2118243800"/>
+        <c:axId val="2062767720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1868,7 +1864,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2120773768"/>
+        <c:crossAx val="2062773320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2072,11 +2068,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2121216360"/>
-        <c:axId val="2121221496"/>
+        <c:axId val="2062734728"/>
+        <c:axId val="2062729128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2121216360"/>
+        <c:axId val="2062734728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2112,12 +2108,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121221496"/>
+        <c:crossAx val="2062729128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2121221496"/>
+        <c:axId val="2062729128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2147,7 +2143,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121216360"/>
+        <c:crossAx val="2062734728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2348,11 +2344,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2120055688"/>
-        <c:axId val="2120060520"/>
+        <c:axId val="2062695992"/>
+        <c:axId val="2062690408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2120055688"/>
+        <c:axId val="2062695992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2388,12 +2384,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2120060520"/>
+        <c:crossAx val="2062690408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2120060520"/>
+        <c:axId val="2062690408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2423,7 +2419,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2120055688"/>
+        <c:crossAx val="2062695992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2612,16 +2608,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>137886</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>36288</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>14515</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>762001</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>72575</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>776516</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>87089</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3087,11 +3083,11 @@
         <v>20</v>
       </c>
       <c r="B4">
-        <f>A4</f>
+        <f t="shared" ref="B4:B15" si="0">A4</f>
         <v>20</v>
       </c>
       <c r="C4">
-        <f>A4</f>
+        <f t="shared" ref="C4:C15" si="1">A4</f>
         <v>20</v>
       </c>
       <c r="D4">
@@ -3113,15 +3109,15 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <f>A5</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C5">
-        <f>A5</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="D5">
-        <f>(5.5-0.1)/0.025</f>
+        <f t="shared" ref="D5:D15" si="2">(5.5-0.1)/0.025</f>
         <v>216</v>
       </c>
       <c r="E5">
@@ -3151,15 +3147,15 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <f>A6</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="C6">
-        <f>A6</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="D6">
-        <f>(5.5-0.1)/0.025</f>
+        <f t="shared" si="2"/>
         <v>216</v>
       </c>
       <c r="E6">
@@ -3189,15 +3185,15 @@
         <v>15</v>
       </c>
       <c r="B7">
-        <f>A7</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="C7">
-        <f>A7</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="D7">
-        <f>(5.5-0.1)/0.025</f>
+        <f t="shared" si="2"/>
         <v>216</v>
       </c>
       <c r="E7">
@@ -3227,15 +3223,15 @@
         <v>20</v>
       </c>
       <c r="B8">
-        <f>A8</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="C8">
-        <f>A8</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="D8">
-        <f>(5.5-0.1)/0.025</f>
+        <f t="shared" si="2"/>
         <v>216</v>
       </c>
       <c r="E8">
@@ -3265,15 +3261,15 @@
         <v>25</v>
       </c>
       <c r="B9">
-        <f>A9</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="C9">
-        <f>A9</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="D9">
-        <f>(5.5-0.1)/0.025</f>
+        <f t="shared" si="2"/>
         <v>216</v>
       </c>
       <c r="E9">
@@ -3303,15 +3299,15 @@
         <v>30</v>
       </c>
       <c r="B10">
-        <f>A10</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="C10">
-        <f>A10</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="D10">
-        <f>(5.5-0.1)/0.025</f>
+        <f t="shared" si="2"/>
         <v>216</v>
       </c>
       <c r="E10">
@@ -3341,15 +3337,15 @@
         <v>35</v>
       </c>
       <c r="B11">
-        <f>A11</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="C11">
-        <f>A11</f>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="D11">
-        <f>(5.5-0.1)/0.025</f>
+        <f t="shared" si="2"/>
         <v>216</v>
       </c>
       <c r="E11">
@@ -3379,15 +3375,15 @@
         <v>40</v>
       </c>
       <c r="B12">
-        <f>A12</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="C12">
-        <f>A12</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="D12">
-        <f>(5.5-0.1)/0.025</f>
+        <f t="shared" si="2"/>
         <v>216</v>
       </c>
       <c r="E12">
@@ -3417,15 +3413,15 @@
         <v>45</v>
       </c>
       <c r="B13">
-        <f>A13</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="C13">
-        <f>A13</f>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="D13">
-        <f>(5.5-0.1)/0.025</f>
+        <f t="shared" si="2"/>
         <v>216</v>
       </c>
       <c r="E13">
@@ -3455,15 +3451,15 @@
         <v>50</v>
       </c>
       <c r="B14">
-        <f>A14</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="C14">
-        <f>A14</f>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="D14">
-        <f>(5.5-0.1)/0.025</f>
+        <f t="shared" si="2"/>
         <v>216</v>
       </c>
       <c r="E14">
@@ -3493,15 +3489,15 @@
         <v>55</v>
       </c>
       <c r="B15">
-        <f>A15</f>
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="C15">
-        <f>A15</f>
+        <f t="shared" si="1"/>
         <v>55</v>
       </c>
       <c r="D15">
-        <f>(5.5-0.1)/0.025</f>
+        <f t="shared" si="2"/>
         <v>216</v>
       </c>
       <c r="E15">
@@ -3531,15 +3527,15 @@
         <v>4</v>
       </c>
       <c r="B17">
-        <f>A17</f>
+        <f t="shared" ref="B17:B23" si="3">A17</f>
         <v>4</v>
       </c>
       <c r="C17">
-        <f>A17</f>
+        <f t="shared" ref="C17:C23" si="4">A17</f>
         <v>4</v>
       </c>
       <c r="D17">
-        <f>(5.5-0.1)/0.001</f>
+        <f t="shared" ref="D17:D22" si="5">(5.5-0.1)/0.001</f>
         <v>5400</v>
       </c>
       <c r="E17">
@@ -3557,15 +3553,15 @@
         <v>10</v>
       </c>
       <c r="B18">
-        <f>A18</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="C18">
-        <f>A18</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="D18">
-        <f>(5.5-0.1)/0.001</f>
+        <f t="shared" si="5"/>
         <v>5400</v>
       </c>
       <c r="E18">
@@ -3583,15 +3579,15 @@
         <v>15</v>
       </c>
       <c r="B19">
-        <f>A19</f>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="C19">
-        <f>A19</f>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="D19">
-        <f>(5.5-0.1)/0.001</f>
+        <f t="shared" si="5"/>
         <v>5400</v>
       </c>
       <c r="E19">
@@ -3609,15 +3605,15 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <f>A20</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="C20">
-        <f>A20</f>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="D20">
-        <f>(5.5-0.1)/0.001</f>
+        <f t="shared" si="5"/>
         <v>5400</v>
       </c>
       <c r="E20">
@@ -3635,15 +3631,15 @@
         <v>25</v>
       </c>
       <c r="B21">
-        <f>A21</f>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="C21">
-        <f>A21</f>
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="D21">
-        <f>(5.5-0.1)/0.001</f>
+        <f t="shared" si="5"/>
         <v>5400</v>
       </c>
       <c r="E21">
@@ -3664,15 +3660,15 @@
         <v>30</v>
       </c>
       <c r="B22">
-        <f>A22</f>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="C22">
-        <f>A22</f>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="D22">
-        <f>(5.5-0.1)/0.001</f>
+        <f t="shared" si="5"/>
         <v>5400</v>
       </c>
       <c r="E22" t="s">
@@ -3690,11 +3686,11 @@
     </row>
     <row r="23" spans="1:8">
       <c r="B23">
-        <f>A23</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="C23">
-        <f>A23</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3721,10 +3717,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3736,12 +3732,20 @@
     <col min="9" max="9" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="2" spans="1:11">
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -3766,21 +3770,30 @@
       <c r="H3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4">
-        <f>A4</f>
+        <f t="shared" ref="B4:B19" si="0">A4</f>
         <v>4</v>
       </c>
       <c r="C4">
-        <f>A4</f>
+        <f t="shared" ref="C4:C19" si="1">A4</f>
         <v>4</v>
       </c>
       <c r="D4">
-        <f>(5.5-0.1)/0.025</f>
+        <f t="shared" ref="D4:D19" si="2">(5.5-0.1)/0.025</f>
         <v>216</v>
       </c>
       <c r="E4">
@@ -3795,21 +3808,33 @@
       <c r="H4">
         <v>1.2803099999999999E-4</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4">
+        <f>F4*$I$2</f>
+        <v>11.697100000000001</v>
+      </c>
+      <c r="J4">
+        <f>I4/60</f>
+        <v>0.19495166666666669</v>
+      </c>
+      <c r="K4">
+        <f>J4/60</f>
+        <v>3.2491944444444447E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>10</v>
       </c>
       <c r="B5">
-        <f>A5</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="C5">
-        <f>A5</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="D5">
-        <f>(5.5-0.1)/0.025</f>
+        <f t="shared" si="2"/>
         <v>216</v>
       </c>
       <c r="E5">
@@ -3824,38 +3849,62 @@
       <c r="H5">
         <v>9.4604499999999996E-4</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5">
+        <f t="shared" ref="I5:I18" si="3">F5*$I$2</f>
+        <v>13.506000000000002</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ref="J5:K18" si="4">I5/60</f>
+        <v>0.22510000000000002</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="4"/>
+        <v>3.751666666666667E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>15</v>
       </c>
       <c r="B6">
-        <f>A6</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="C6">
-        <f>A6</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="D6">
-        <f>(5.5-0.1)/0.025</f>
+        <f t="shared" si="2"/>
         <v>216</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>20</v>
       </c>
       <c r="B7">
-        <f>A7</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="C7">
-        <f>A7</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="D7">
-        <f>(5.5-0.1)/0.025</f>
+        <f t="shared" si="2"/>
         <v>216</v>
       </c>
       <c r="E7">
@@ -3870,38 +3919,62 @@
       <c r="H7">
         <v>2.6683999999999999E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7">
+        <f t="shared" si="3"/>
+        <v>24.9129</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="4"/>
+        <v>0.415215</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="4"/>
+        <v>6.9202500000000002E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>25</v>
       </c>
       <c r="B8">
-        <f>A8</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="C8">
-        <f>A8</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="D8">
-        <f>(5.5-0.1)/0.025</f>
+        <f t="shared" si="2"/>
         <v>216</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>30</v>
       </c>
       <c r="B9">
-        <f>A9</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="C9">
-        <f>A9</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="D9">
-        <f>(5.5-0.1)/0.025</f>
+        <f t="shared" si="2"/>
         <v>216</v>
       </c>
       <c r="E9">
@@ -3916,38 +3989,62 @@
       <c r="H9">
         <v>0.16317599999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9">
+        <f t="shared" si="3"/>
+        <v>60.2958</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="4"/>
+        <v>1.0049300000000001</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="4"/>
+        <v>1.6748833333333334E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>35</v>
       </c>
       <c r="B10">
-        <f>A10</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="C10">
-        <f>A10</f>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="D10">
-        <f>(5.5-0.1)/0.025</f>
+        <f t="shared" si="2"/>
         <v>216</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11">
         <v>40</v>
       </c>
       <c r="B11">
-        <f>A11</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="C11">
-        <f>A11</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="D11">
-        <f>(5.5-0.1)/0.025</f>
+        <f t="shared" si="2"/>
         <v>216</v>
       </c>
       <c r="E11">
@@ -3962,38 +4059,62 @@
       <c r="H11">
         <v>0.63618600000000003</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11">
+        <f t="shared" si="3"/>
+        <v>169.721</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="4"/>
+        <v>2.8286833333333332</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="4"/>
+        <v>4.714472222222222E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12">
         <v>45</v>
       </c>
       <c r="B12">
-        <f>A12</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="C12">
-        <f>A12</f>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="D12">
-        <f>(5.5-0.1)/0.025</f>
+        <f t="shared" si="2"/>
         <v>216</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="I12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13">
         <v>50</v>
       </c>
       <c r="B13">
-        <f>A13</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="C13">
-        <f>A13</f>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="D13">
-        <f>(5.5-0.1)/0.025</f>
+        <f t="shared" si="2"/>
         <v>216</v>
       </c>
       <c r="E13">
@@ -4008,21 +4129,33 @@
       <c r="H13">
         <v>2.07382</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="I13">
+        <f t="shared" si="3"/>
+        <v>434.71599999999995</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="4"/>
+        <v>7.2452666666666659</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="4"/>
+        <v>0.12075444444444443</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14">
         <v>60</v>
       </c>
       <c r="B14">
-        <f>A14</f>
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="C14">
-        <f>A14</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="D14">
-        <f>(5.5-0.1)/0.025</f>
+        <f t="shared" si="2"/>
         <v>216</v>
       </c>
       <c r="E14">
@@ -4037,21 +4170,33 @@
       <c r="H14">
         <v>5.46896</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="I14">
+        <f t="shared" si="3"/>
+        <v>992.26899999999989</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="4"/>
+        <v>16.537816666666664</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="4"/>
+        <v>0.27563027777777777</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15">
         <v>70</v>
       </c>
       <c r="B15">
-        <f>A15</f>
+        <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="C15">
-        <f>A15</f>
+        <f t="shared" si="1"/>
         <v>70</v>
       </c>
       <c r="D15">
-        <f>(5.5-0.1)/0.025</f>
+        <f t="shared" si="2"/>
         <v>216</v>
       </c>
       <c r="E15">
@@ -4066,21 +4211,33 @@
       <c r="H15">
         <v>12.7608</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="I15">
+        <f t="shared" si="3"/>
+        <v>2078.3200000000002</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="4"/>
+        <v>34.638666666666673</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="4"/>
+        <v>0.57731111111111122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16">
         <v>100</v>
       </c>
       <c r="B16">
-        <f>A16</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="C16">
-        <f>A16</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="D16">
-        <f>(5.5-0.1)/0.025</f>
+        <f t="shared" si="2"/>
         <v>216</v>
       </c>
       <c r="E16">
@@ -4095,21 +4252,33 @@
       <c r="H16">
         <v>91.689400000000006</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="I16">
+        <f t="shared" si="3"/>
+        <v>12415.5</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="4"/>
+        <v>206.92500000000001</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="4"/>
+        <v>3.44875</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17">
         <v>120</v>
       </c>
       <c r="B17">
-        <f>A17</f>
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
       <c r="C17">
-        <f>A17</f>
+        <f t="shared" si="1"/>
         <v>120</v>
       </c>
       <c r="D17">
-        <f>(5.5-0.1)/0.025</f>
+        <f t="shared" si="2"/>
         <v>216</v>
       </c>
       <c r="E17">
@@ -4124,21 +4293,33 @@
       <c r="H17">
         <v>280.09399999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="I17">
+        <f t="shared" si="3"/>
+        <v>34792.300000000003</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="4"/>
+        <v>579.87166666666667</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="4"/>
+        <v>9.6645277777777778</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18">
         <v>130</v>
       </c>
       <c r="B18">
-        <f>A18</f>
+        <f t="shared" si="0"/>
         <v>130</v>
       </c>
       <c r="C18">
-        <f>A18</f>
+        <f t="shared" si="1"/>
         <v>130</v>
       </c>
       <c r="D18">
-        <f>(5.5-0.1)/0.025</f>
+        <f t="shared" si="2"/>
         <v>216</v>
       </c>
       <c r="F18">
@@ -4150,137 +4331,149 @@
       <c r="H18">
         <v>453.03699999999998</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="I18">
+        <f t="shared" si="3"/>
+        <v>54827.9</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="4"/>
+        <v>913.7983333333334</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="4"/>
+        <v>15.229972222222223</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19">
         <v>150</v>
       </c>
       <c r="B19">
-        <f>A19</f>
+        <f t="shared" si="0"/>
         <v>150</v>
       </c>
       <c r="C19">
-        <f>A19</f>
+        <f t="shared" si="1"/>
         <v>150</v>
       </c>
       <c r="D19">
-        <f>(5.5-0.1)/0.025</f>
+        <f t="shared" si="2"/>
         <v>216</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:11">
       <c r="A21">
         <v>4</v>
       </c>
       <c r="B21">
-        <f>A21</f>
+        <f t="shared" ref="B21:B27" si="5">A21</f>
         <v>4</v>
       </c>
       <c r="C21">
-        <f>A21</f>
+        <f t="shared" ref="C21:C27" si="6">A21</f>
         <v>4</v>
       </c>
       <c r="D21">
-        <f>(5.5-0.1)/0.001</f>
+        <f t="shared" ref="D21:D26" si="7">(5.5-0.1)/0.001</f>
         <v>5400</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:11">
       <c r="A22">
         <v>10</v>
       </c>
       <c r="B22">
-        <f>A22</f>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="C22">
-        <f>A22</f>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="D22">
-        <f>(5.5-0.1)/0.001</f>
+        <f t="shared" si="7"/>
         <v>5400</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:11">
       <c r="A23">
         <v>15</v>
       </c>
       <c r="B23">
-        <f>A23</f>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="C23">
-        <f>A23</f>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="D23">
-        <f>(5.5-0.1)/0.001</f>
+        <f t="shared" si="7"/>
         <v>5400</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:11">
       <c r="A24">
         <v>20</v>
       </c>
       <c r="B24">
-        <f>A24</f>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
       <c r="C24">
-        <f>A24</f>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="D24">
-        <f>(5.5-0.1)/0.001</f>
+        <f t="shared" si="7"/>
         <v>5400</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:11">
       <c r="A25">
         <v>25</v>
       </c>
       <c r="B25">
-        <f>A25</f>
+        <f t="shared" si="5"/>
         <v>25</v>
       </c>
       <c r="C25">
-        <f>A25</f>
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
       <c r="D25">
-        <f>(5.5-0.1)/0.001</f>
+        <f t="shared" si="7"/>
         <v>5400</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:11">
       <c r="A26">
         <v>30</v>
       </c>
       <c r="B26">
-        <f>A26</f>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="C26">
-        <f>A26</f>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
       <c r="D26">
-        <f>(5.5-0.1)/0.001</f>
+        <f t="shared" si="7"/>
         <v>5400</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:11">
       <c r="B27">
-        <f>A27</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="C27">
-        <f>A27</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:11">
       <c r="A29" t="s">
         <v>13</v>
       </c>

</xml_diff>